<commit_message>
change load resistor values at R2R output to have a more colourful picture
</commit_message>
<xml_diff>
--- a/generalRGBmod/Main-PCB/BOM_n64rgb.xlsx
+++ b/generalRGBmod/Main-PCB/BOM_n64rgb.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Documents\Workspaces\Git\n64rgb\generalRGBmod\Main-PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/Git/N64RGB/generalRGBmod/Main-PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="MaxV Setup" sheetId="1" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>CAT16-1001F4LF</t>
   </si>
   <si>
-    <t>CRCW0603270RFKEAH</t>
-  </si>
-  <si>
     <t>RN20</t>
   </si>
   <si>
@@ -351,9 +348,6 @@
     <t>4x 39ohm (1%)</t>
   </si>
   <si>
-    <t>270ohm (1%)</t>
-  </si>
-  <si>
     <t>Short J1</t>
   </si>
   <si>
@@ -367,12 +361,18 @@
   </si>
   <si>
     <t>Alternative to 5M570ZT100 with less LEs</t>
+  </si>
+  <si>
+    <t>280ohm (1%)</t>
+  </si>
+  <si>
+    <t>RC0603FR-07280RL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -917,17 +917,17 @@
     <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1215,18 +1215,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1249,13 +1249,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1285,12 +1285,12 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>25</v>
@@ -1330,7 +1330,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1368,7 +1368,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1379,7 +1379,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>37</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>42</v>
       </c>
@@ -1468,18 +1468,18 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1523,7 +1523,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1548,7 +1548,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1570,7 +1570,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1592,7 +1592,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" t="s">
         <v>54</v>
@@ -1614,15 +1614,15 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -1633,7 +1633,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -1655,7 +1655,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -1677,7 +1677,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -1699,7 +1699,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
         <v>11</v>
@@ -1721,7 +1721,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" t="s">
         <v>11</v>
@@ -1743,13 +1743,13 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="7"/>
       <c r="E30" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
@@ -1757,7 +1757,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -1768,10 +1768,10 @@
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1779,7 +1779,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -1790,10 +1790,10 @@
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1802,12 +1802,12 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C33" s="7">
         <v>3</v>
@@ -1816,7 +1816,7 @@
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -1825,55 +1825,55 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
         <v>89</v>
-      </c>
-      <c r="B34" t="s">
-        <v>90</v>
       </c>
       <c r="C34" s="7">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>16</v>
       </c>
@@ -1886,60 +1886,60 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E45" s="3"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E46" s="3"/>
       <c r="G46" s="2"/>
       <c r="H46" s="4"/>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="4"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
     </row>
   </sheetData>
@@ -1955,18 +1955,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1989,18 +1989,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2014,9 +2014,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -2025,12 +2025,12 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -2051,7 +2051,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>25</v>
@@ -2070,7 +2070,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
@@ -2080,16 +2080,16 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2100,7 +2100,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2135,7 +2135,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>43</v>
       </c>
@@ -2151,7 +2151,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>42</v>
       </c>
@@ -2189,18 +2189,18 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E20" t="s">
         <v>54</v>
@@ -2291,15 +2291,15 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -2310,7 +2310,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -2332,7 +2332,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -2354,7 +2354,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
@@ -2376,7 +2376,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -2398,7 +2398,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -2420,13 +2420,13 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>85</v>
       </c>
       <c r="C27" s="7"/>
       <c r="E27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -2434,7 +2434,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -2445,10 +2445,10 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -2456,7 +2456,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -2467,10 +2467,10 @@
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -2479,12 +2479,12 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C30" s="7">
         <v>3</v>
@@ -2493,7 +2493,7 @@
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
@@ -2502,55 +2502,55 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
         <v>89</v>
-      </c>
-      <c r="B31" t="s">
-        <v>90</v>
       </c>
       <c r="C31" s="7">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>16</v>
       </c>
@@ -2563,60 +2563,60 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E40" s="3"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="4"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="4"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
     </row>
   </sheetData>

</xml_diff>